<commit_message>
update songlist level change
</commit_message>
<xml_diff>
--- a/docs/songlist/songlist.xlsx
+++ b/docs/songlist/songlist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clarilotus\github\ez2on\docs\songlist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F42D3ED-ADC6-44FC-B6E3-29C43A268373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762AB250-2A81-49A5-8D90-CBFB8EEB16D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4155,10 +4155,10 @@
   <dimension ref="A1:AM392"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="V102" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomRight" activeCell="AI128" sqref="A1:AM392"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -8399,7 +8399,7 @@
         <v>15</v>
       </c>
       <c r="T36" s="6">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="U36" s="6">
         <v>8</v>
@@ -19112,7 +19112,7 @@
         <v>7</v>
       </c>
       <c r="U126" s="6">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="V126" s="6">
         <v>15</v>
@@ -19160,7 +19160,7 @@
         <v>7</v>
       </c>
       <c r="AK126" s="11">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AL126" s="11">
         <v>15</v>
@@ -25270,7 +25270,7 @@
         <v>13</v>
       </c>
       <c r="K178" s="6">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L178" s="6">
         <v>5</v>
@@ -25318,7 +25318,7 @@
         <v>13</v>
       </c>
       <c r="AA178" s="8">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AB178" s="9">
         <v>5</v>
@@ -25892,7 +25892,7 @@
         <v>15</v>
       </c>
       <c r="T183" s="6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="U183" s="6">
         <v>10</v>
@@ -25940,7 +25940,7 @@
         <v>15</v>
       </c>
       <c r="AJ183" s="11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AK183" s="11">
         <v>10</v>
@@ -29572,7 +29572,7 @@
         <v>5</v>
       </c>
       <c r="Q214" s="6">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="R214" s="6">
         <v>14</v>
@@ -29620,7 +29620,7 @@
         <v>5</v>
       </c>
       <c r="AG214" s="10">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AH214" s="10">
         <v>14</v>
@@ -38476,7 +38476,7 @@
         <v>11</v>
       </c>
       <c r="J289" s="6">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K289" s="6">
         <v>19</v>
@@ -38524,7 +38524,7 @@
         <v>11</v>
       </c>
       <c r="Z289" s="8">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AA289" s="8">
         <v>19</v>
@@ -39190,7 +39190,7 @@
         <v>9</v>
       </c>
       <c r="J295" s="6">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K295" s="6">
         <v>17</v>
@@ -39238,7 +39238,7 @@
         <v>9</v>
       </c>
       <c r="Z295" s="8">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AA295" s="8">
         <v>17</v>
@@ -40859,7 +40859,7 @@
         <v>12</v>
       </c>
       <c r="K309" s="6">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L309" s="6">
         <v>4</v>
@@ -40907,7 +40907,7 @@
         <v>12</v>
       </c>
       <c r="AA309" s="8">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AB309" s="9">
         <v>4</v>
@@ -41341,10 +41341,10 @@
         <v>7</v>
       </c>
       <c r="M313" s="6">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N313" s="6">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O313" s="6">
         <v>20</v>
@@ -41353,10 +41353,10 @@
         <v>7</v>
       </c>
       <c r="Q313" s="6">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="R313" s="6">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="S313" s="6">
         <v>20</v>
@@ -41389,10 +41389,10 @@
         <v>7</v>
       </c>
       <c r="AC313" s="9">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AD313" s="9">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AE313" s="9">
         <v>20</v>
@@ -41401,10 +41401,10 @@
         <v>7</v>
       </c>
       <c r="AG313" s="10">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AH313" s="10">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AI313" s="10">
         <v>20</v>
@@ -47065,7 +47065,7 @@
         <v>14</v>
       </c>
       <c r="S361" s="6">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="T361" s="6">
         <v>4</v>
@@ -47113,7 +47113,7 @@
         <v>14</v>
       </c>
       <c r="AI361" s="10">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AJ361" s="11">
         <v>7</v>
@@ -47425,7 +47425,7 @@
         <v>12</v>
       </c>
       <c r="V364" s="6">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="W364" s="6">
         <v>18</v>
@@ -47473,7 +47473,7 @@
         <v>12</v>
       </c>
       <c r="AL364" s="11">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AM364" s="11">
         <v>18</v>
@@ -48447,7 +48447,7 @@
         <v>14</v>
       </c>
       <c r="K373" s="6">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L373" s="6">
         <v>4</v>
@@ -48495,7 +48495,7 @@
         <v>14</v>
       </c>
       <c r="AA373" s="8">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AB373" s="9">
         <v>4</v>

</xml_diff>

<commit_message>
update 23fd course info and snow dream remaster
</commit_message>
<xml_diff>
--- a/docs/songlist/songlist.xlsx
+++ b/docs/songlist/songlist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clarilotus\GitHub\ez2on\docs\songlist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7480386-72DF-47CE-B4E0-F4BF47A68C45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13BDE827-DEEF-43B0-BAE2-728B4D72AD0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2047" uniqueCount="1090">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2047" uniqueCount="1091">
   <si>
     <t>1ST</t>
   </si>
@@ -3498,6 +3498,10 @@
   </si>
   <si>
     <t>Snow Dream (Ramaster)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SIGMA</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -4815,10 +4819,10 @@
   <dimension ref="A1:AM430"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D86" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D201" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H32" sqref="H32"/>
+      <selection pane="bottomRight" activeCell="I219" sqref="I219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -30737,7 +30741,7 @@
         <v>2013</v>
       </c>
       <c r="C219" s="27" t="s">
-        <v>475</v>
+        <v>1090</v>
       </c>
       <c r="D219" s="27" t="s">
         <v>475</v>
@@ -30987,38 +30991,102 @@
         <v>133</v>
       </c>
       <c r="G221" s="2"/>
-      <c r="H221" s="4"/>
-      <c r="I221" s="4"/>
-      <c r="J221" s="4"/>
-      <c r="K221" s="4"/>
-      <c r="L221" s="4"/>
-      <c r="M221" s="4"/>
-      <c r="N221" s="4"/>
-      <c r="O221" s="4"/>
-      <c r="P221" s="4"/>
-      <c r="Q221" s="4"/>
-      <c r="R221" s="4"/>
-      <c r="S221" s="4"/>
-      <c r="T221" s="4"/>
-      <c r="U221" s="4"/>
-      <c r="V221" s="4"/>
-      <c r="W221" s="4"/>
-      <c r="X221" s="5"/>
-      <c r="Y221" s="5"/>
-      <c r="Z221" s="5"/>
-      <c r="AA221" s="5"/>
-      <c r="AB221" s="6"/>
-      <c r="AC221" s="6"/>
-      <c r="AD221" s="6"/>
-      <c r="AE221" s="6"/>
-      <c r="AF221" s="7"/>
-      <c r="AG221" s="7"/>
-      <c r="AH221" s="7"/>
-      <c r="AI221" s="7"/>
-      <c r="AJ221" s="8"/>
-      <c r="AK221" s="8"/>
-      <c r="AL221" s="8"/>
-      <c r="AM221" s="8"/>
+      <c r="H221" s="4">
+        <v>4</v>
+      </c>
+      <c r="I221" s="4">
+        <v>9</v>
+      </c>
+      <c r="J221" s="4">
+        <v>13</v>
+      </c>
+      <c r="K221" s="4">
+        <v>15</v>
+      </c>
+      <c r="L221" s="4">
+        <v>3</v>
+      </c>
+      <c r="M221" s="4">
+        <v>7</v>
+      </c>
+      <c r="N221" s="4">
+        <v>12</v>
+      </c>
+      <c r="O221" s="4">
+        <v>15</v>
+      </c>
+      <c r="P221" s="4">
+        <v>4</v>
+      </c>
+      <c r="Q221" s="4">
+        <v>9</v>
+      </c>
+      <c r="R221" s="4">
+        <v>13</v>
+      </c>
+      <c r="S221" s="4">
+        <v>15</v>
+      </c>
+      <c r="T221" s="4">
+        <v>4</v>
+      </c>
+      <c r="U221" s="4">
+        <v>8</v>
+      </c>
+      <c r="V221" s="4">
+        <v>13</v>
+      </c>
+      <c r="W221" s="4">
+        <v>16</v>
+      </c>
+      <c r="X221" s="5">
+        <v>4</v>
+      </c>
+      <c r="Y221" s="5">
+        <v>9</v>
+      </c>
+      <c r="Z221" s="5">
+        <v>13</v>
+      </c>
+      <c r="AA221" s="5">
+        <v>15</v>
+      </c>
+      <c r="AB221" s="6">
+        <v>3</v>
+      </c>
+      <c r="AC221" s="6">
+        <v>7</v>
+      </c>
+      <c r="AD221" s="6">
+        <v>12</v>
+      </c>
+      <c r="AE221" s="6">
+        <v>15</v>
+      </c>
+      <c r="AF221" s="7">
+        <v>4</v>
+      </c>
+      <c r="AG221" s="7">
+        <v>9</v>
+      </c>
+      <c r="AH221" s="7">
+        <v>13</v>
+      </c>
+      <c r="AI221" s="7">
+        <v>15</v>
+      </c>
+      <c r="AJ221" s="8">
+        <v>4</v>
+      </c>
+      <c r="AK221" s="8">
+        <v>8</v>
+      </c>
+      <c r="AL221" s="8">
+        <v>13</v>
+      </c>
+      <c r="AM221" s="8">
+        <v>16</v>
+      </c>
     </row>
     <row r="222" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A222" s="57">

</xml_diff>